<commit_message>
Add Presentation Chunk to awesomeCV_amb
</commit_message>
<xml_diff>
--- a/awesomecv_amb/CVdata.xlsx
+++ b/awesomecv_amb/CVdata.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burns/Documents/Github/CurriculumVitae/awesomecv_amb/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0501AD6-B250-2F48-840F-7C9A40569939}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="12160" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Experience" sheetId="1" r:id="rId1"/>
-    <sheet name="Teaching" sheetId="4" r:id="rId2"/>
-    <sheet name="Extracurriculars" sheetId="5" r:id="rId3"/>
-    <sheet name="References" sheetId="2" r:id="rId4"/>
-    <sheet name="Skills" sheetId="6" r:id="rId5"/>
-    <sheet name="Certificates" sheetId="7" r:id="rId6"/>
-    <sheet name="Presentations" sheetId="8" r:id="rId7"/>
+    <sheet name="Education" sheetId="9" r:id="rId1"/>
+    <sheet name="Experience" sheetId="1" r:id="rId2"/>
+    <sheet name="Teaching" sheetId="4" r:id="rId3"/>
+    <sheet name="Presentations" sheetId="8" r:id="rId4"/>
+    <sheet name="Extracurriculars" sheetId="5" r:id="rId5"/>
+    <sheet name="References" sheetId="2" r:id="rId6"/>
+    <sheet name="Skills" sheetId="6" r:id="rId7"/>
+    <sheet name="Certificates" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="110">
   <si>
     <t>Title</t>
   </si>
@@ -355,11 +362,86 @@
   <si>
     <t>LTK certificate</t>
   </si>
+  <si>
+    <t>role-title</t>
+  </si>
+  <si>
+    <t>department-name</t>
+  </si>
+  <si>
+    <t>end-date.year.value</t>
+  </si>
+  <si>
+    <t>organization.name</t>
+  </si>
+  <si>
+    <t>organization.address.city</t>
+  </si>
+  <si>
+    <t>organization.address.region</t>
+  </si>
+  <si>
+    <t>organization.address.country</t>
+  </si>
+  <si>
+    <t>thesis</t>
+  </si>
+  <si>
+    <t>Testing the theory of Epigenetic Priming in Fear Memory Conditioning</t>
+  </si>
+  <si>
+    <t>Effects of the splicing inhibitor, Isoginkgetin, on human Telomerase RNA</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Switerland</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Neuroscience</t>
+  </si>
+  <si>
+    <t>École Polytechnique Fédérale de Lausanne</t>
+  </si>
+  <si>
+    <t>Ph.D</t>
+  </si>
+  <si>
+    <t>Eugene</t>
+  </si>
+  <si>
+    <t>M.Sc</t>
+  </si>
+  <si>
+    <t>B.Sc</t>
+  </si>
+  <si>
+    <t>Bioinformatics</t>
+  </si>
+  <si>
+    <t>Biology, Minor in Chemistry</t>
+  </si>
+  <si>
+    <t>Chicago, Illinois</t>
+  </si>
+  <si>
+    <t>Symposium</t>
+  </si>
+  <si>
+    <t>MCCS 2019</t>
+  </si>
+  <si>
+    <t>Oct. 18, 2019</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -661,6 +743,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -985,14 +1075,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20407B7-9BD7-0846-A55F-6E579A78E032}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" customWidth="1"/>
+    <col min="2" max="4" width="20.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3">
+        <v>2013</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4">
+        <v>2012</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="36.33203125" style="1" customWidth="1"/>
@@ -1005,7 +1215,7 @@
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1241,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1057,7 +1267,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1083,7 +1293,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1109,7 +1319,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1135,7 +1345,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1161,7 +1371,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1187,7 +1397,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1213,7 +1423,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1239,7 +1449,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1265,7 +1475,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1291,7 +1501,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1317,7 +1527,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1343,7 +1553,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1369,7 +1579,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1393,108 +1603,6 @@
       </c>
       <c r="H15" s="4" t="s">
         <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="44.1640625" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1509,61 +1617,94 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="44.1640625" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>54</v>
+      </c>
+      <c r="C3">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1578,67 +1719,43 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.83203125" customWidth="1"/>
-    <col min="2" max="2" width="73" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>46</v>
+        <v>109</v>
+      </c>
+      <c r="C2" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1648,50 +1765,61 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>83</v>
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1706,22 +1834,67 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="52.83203125" customWidth="1"/>
+    <col min="2" max="2" width="73" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1731,13 +1904,82 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>